<commit_message>
Latest Commit for 05-03-2020
</commit_message>
<xml_diff>
--- a/Solar Curtailment/Backup Files/ChangedDatafor470row.xlsx
+++ b/Solar Curtailment/Backup Files/ChangedDatafor470row.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="570" windowWidth="20775" windowHeight="9150"/>
+    <workbookView xWindow="390" yWindow="570" windowWidth="20775" windowHeight="9150" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Talarichruvu" sheetId="4" r:id="rId4"/>
     <sheet name="Mylavaram" sheetId="5" r:id="rId5"/>
     <sheet name="All Stations" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6058" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6070" uniqueCount="693">
   <si>
     <t>Date</t>
   </si>
@@ -2476,8 +2477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A511" workbookViewId="0">
+      <selection activeCell="A527" sqref="A527:XFD527"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -102520,4 +102521,95 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="1">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2">
+        <v>120</v>
+      </c>
+      <c r="F2">
+        <v>150</v>
+      </c>
+      <c r="G2">
+        <v>592</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="1">
+        <v>525</v>
+      </c>
+      <c r="B3" t="s">
+        <v>435</v>
+      </c>
+      <c r="C3">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>439</v>
+      </c>
+      <c r="E3" s="2">
+        <v>-100</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <v>679</v>
+      </c>
+      <c r="H3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>